<commit_message>
Excel Feature: Small bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelActivityWithLinksTest.xlsx
+++ b/src/test/resources/visitExcelActivityWithLinksTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50B3B36-FE75-4B05-8CE5-8A32DE5EA3C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF2C0C-DF98-4B22-8C51-899C75172975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -561,6 +561,18 @@
   </si>
   <si>
     <t>place</t>
+  </si>
+  <si>
+    <t>Person1</t>
+  </si>
+  <si>
+    <t>Person2</t>
+  </si>
+  <si>
+    <t>Seite</t>
+  </si>
+  <si>
+    <t>Links</t>
   </si>
 </sst>
 </file>
@@ -2979,7 +2991,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2999,36 +3011,57 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>162</v>
       </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>163</v>
       </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:2" s="137" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="137" t="s">
@@ -3039,19 +3072,31 @@
       <c r="A10" s="138" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="138" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:2" s="139" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="139" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="139" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>